<commit_message>
SSDM-13693: Made sample and experiment visible in default export of datasets.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-filtered-fields.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-filtered-fields.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">TEST_2</t>
   </si>
   <si>
-    <t xml:space="preserve">/TEST/TEST_2</t>
+    <t xml:space="preserve">/TEST/TEST/TEST_2</t>
   </si>
   <si>
     <t xml:space="preserve">file1.bin</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">TEST_3</t>
   </si>
   <si>
-    <t xml:space="preserve">/TEST/TEST_3</t>
+    <t xml:space="preserve">/TEST/TEST/TEST_3</t>
   </si>
   <si>
     <t xml:space="preserve">file2.bin</t>
@@ -263,10 +263,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ12"/>
+  <dimension ref="A1:AMK12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -276,7 +276,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="8.36"/>
   </cols>
@@ -314,6 +314,8 @@
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="G4" s="1"/>
+      <c r="AMI4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -331,6 +333,8 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G5" s="1"/>
+      <c r="AMI5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -348,6 +352,8 @@
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G6" s="1"/>
+      <c r="AMI6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,6 +393,7 @@
         <v>21</v>
       </c>
       <c r="AMJ11" s="1"/>
+      <c r="AMK11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
@@ -407,6 +414,8 @@
       <c r="F12" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="G12" s="1"/>
+      <c r="AMI12" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>